<commit_message>
added parse script to get searchcriteria
</commit_message>
<xml_diff>
--- a/listcommands.xlsx
+++ b/listcommands.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31540" yWindow="5660" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="38660" yWindow="8200" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="10.5" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
   <si>
     <t>list_sip_profile</t>
   </si>
@@ -522,6 +522,9 @@
   </si>
   <si>
     <t>Command</t>
+  </si>
+  <si>
+    <t>searchcriteria</t>
   </si>
 </sst>
 </file>
@@ -836,93 +839,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A166"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>